<commit_message>
Added steps for 15th June 2016
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Month" sheetId="2" r:id="rId1"/>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,19 +719,19 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>171318</v>
+        <v>179580</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>12237</v>
+        <v>11972</v>
       </c>
       <c r="L24" s="1">
         <f>(30*N6)-I24</f>
-        <v>121856.86607142858</v>
+        <v>113594.86607142858</v>
       </c>
       <c r="M24" s="4">
         <f>L24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>6769.8258928571431</v>
+        <v>6310.8258928571431</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -833,6 +833,9 @@
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>42536</v>
+      </c>
+      <c r="B37" s="1">
+        <v>8262</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Jun 19 2016 Steps
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,19 +719,19 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>224808</v>
+        <v>246035</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>12489.333333333334</v>
+        <v>12949.21052631579</v>
       </c>
       <c r="L24" s="1">
         <f>(30*N6)-I24</f>
-        <v>68366.86607142858</v>
+        <v>47139.86607142858</v>
       </c>
       <c r="M24" s="4">
         <f>L24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>3798.1592261904766</v>
+        <v>2618.8814484126988</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -865,6 +865,9 @@
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>42540</v>
+      </c>
+      <c r="B41" s="1">
+        <v>21227</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added June 20 Steps and Modified  A21 to "Date"
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Month</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -531,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,8 +686,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>42522</v>
+      <c r="A21" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -719,19 +722,19 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>246035</v>
+        <v>266968</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>12949.21052631579</v>
+        <v>13348.4</v>
       </c>
       <c r="L24" s="1">
         <f>(30*N6)-I24</f>
-        <v>47139.86607142858</v>
+        <v>26206.86607142858</v>
       </c>
       <c r="M24" s="4">
         <f>L24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>2618.8814484126988</v>
+        <v>1455.9370039682544</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -873,6 +876,9 @@
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>42541</v>
+      </c>
+      <c r="B42" s="1">
+        <v>20933</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added June 22 Steps
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -535,7 +535,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,19 +722,19 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>266968</v>
+        <v>281859</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>13348.4</v>
+        <v>13421.857142857143</v>
       </c>
       <c r="L24" s="1">
         <f>(30*N6)-I24</f>
-        <v>26206.86607142858</v>
+        <v>11315.86607142858</v>
       </c>
       <c r="M24" s="4">
         <f>L24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>1455.9370039682544</v>
+        <v>628.6592261904766</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -884,6 +884,9 @@
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42542</v>
+      </c>
+      <c r="B43" s="1">
+        <v>14891</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added June 22 Steps as well as updated text under columns
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -41,12 +41,6 @@
     <t>Average Daily</t>
   </si>
   <si>
-    <t>So far Daily Average</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Steps </t>
-  </si>
-  <si>
     <t>Remaining Steps for Month</t>
   </si>
   <si>
@@ -60,6 +54,12 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Total Steps  (Current Month)</t>
+  </si>
+  <si>
+    <t>Daily Average (Current Month)</t>
   </si>
 </sst>
 </file>
@@ -534,22 +534,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="41.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="34" style="1" customWidth="1"/>
     <col min="14" max="14" width="21" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>42278</v>
       </c>
@@ -565,7 +566,7 @@
         <v>203619</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42309</v>
       </c>
@@ -573,7 +574,7 @@
         <v>394148</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42339</v>
       </c>
@@ -581,7 +582,7 @@
         <v>240808</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42370</v>
       </c>
@@ -591,14 +592,14 @@
       <c r="J5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42401</v>
       </c>
@@ -606,19 +607,19 @@
         <v>217839</v>
       </c>
       <c r="J6" s="1">
-        <f>AVERAGE(B2:B9)</f>
+        <f>AVERAGE(B2:B16)</f>
         <v>273629.875</v>
       </c>
-      <c r="L6" s="1">
+      <c r="K6" s="1">
         <f>J6/4</f>
         <v>68407.46875</v>
       </c>
-      <c r="N6" s="1">
-        <f>L6/7</f>
+      <c r="L6" s="1">
+        <f>K6/7</f>
         <v>9772.4955357142862</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42430</v>
       </c>
@@ -626,7 +627,7 @@
         <v>229226</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42461</v>
       </c>
@@ -634,7 +635,7 @@
         <v>293270</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42491</v>
       </c>
@@ -642,58 +643,58 @@
         <v>260955</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>42522</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>42552</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42583</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42614</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42644</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42675</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42705</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>42522</v>
       </c>
@@ -701,19 +702,19 @@
         <v>13489</v>
       </c>
       <c r="I23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>42523</v>
       </c>
@@ -722,22 +723,22 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>281859</v>
+        <v>296052</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>13421.857142857143</v>
-      </c>
-      <c r="L24" s="1">
-        <f>(30*N6)-I24</f>
-        <v>11315.86607142858</v>
-      </c>
-      <c r="M24" s="4">
-        <f>L24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>628.6592261904766</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>13456.90909090909</v>
+      </c>
+      <c r="K24" s="1">
+        <f>(30*L6)-I24</f>
+        <v>-2877.1339285714203</v>
+      </c>
+      <c r="L24" s="4">
+        <f>K24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
+        <v>-159.84077380952334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>42524</v>
       </c>
@@ -745,7 +746,7 @@
         <v>8509</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>42525</v>
       </c>
@@ -753,7 +754,7 @@
         <v>18480</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>42526</v>
       </c>
@@ -761,7 +762,7 @@
         <v>4784</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>42527</v>
       </c>
@@ -769,7 +770,7 @@
         <v>21982</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>42528</v>
       </c>
@@ -777,7 +778,7 @@
         <v>15662</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>42529</v>
       </c>
@@ -785,7 +786,7 @@
         <v>6412</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>42530</v>
       </c>
@@ -793,7 +794,7 @@
         <v>7959</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>42531</v>
       </c>
@@ -892,6 +893,9 @@
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>42543</v>
+      </c>
+      <c r="B44" s="1">
+        <v>14193</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added June 23 Steps
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -535,7 +535,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,19 +723,19 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>296052</v>
+        <v>311028</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>13456.90909090909</v>
+        <v>13522.95652173913</v>
       </c>
       <c r="K24" s="1">
         <f>(30*L6)-I24</f>
-        <v>-2877.1339285714203</v>
+        <v>-17853.13392857142</v>
       </c>
       <c r="L24" s="4">
         <f>K24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>-159.84077380952334</v>
+        <v>-991.8407738095234</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -901,6 +901,9 @@
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>42544</v>
+      </c>
+      <c r="B45" s="1">
+        <v>14976</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Jun 24 and June 25th Steps
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -535,7 +535,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,19 +723,19 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>311028</v>
+        <v>335907</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>13522.95652173913</v>
+        <v>13436.28</v>
       </c>
       <c r="K24" s="1">
         <f>(30*L6)-I24</f>
-        <v>-17853.13392857142</v>
+        <v>-42732.13392857142</v>
       </c>
       <c r="L24" s="4">
         <f>K24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>-991.8407738095234</v>
+        <v>-2374.0074404761899</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -910,10 +910,16 @@
       <c r="A46" s="3">
         <v>42545</v>
       </c>
+      <c r="B46" s="1">
+        <v>7515</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>42546</v>
+      </c>
+      <c r="B47" s="1">
+        <v>17364</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added June 26 and June 27 Steps
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -535,7 +535,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,19 +723,19 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>335907</v>
+        <v>352388</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>13436.28</v>
+        <v>13051.407407407407</v>
       </c>
       <c r="K24" s="1">
         <f>(30*L6)-I24</f>
-        <v>-42732.13392857142</v>
+        <v>-59213.13392857142</v>
       </c>
       <c r="L24" s="4">
         <f>K24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>-2374.0074404761899</v>
+        <v>-3289.6185515873012</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -926,23 +926,29 @@
       <c r="A48" s="3">
         <v>42547</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>7425</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>42548</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>9056</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>42549</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>42550</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>42551</v>
       </c>

</xml_diff>

<commit_message>
Updated June 28th and June 29th Steps
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,19 +723,19 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>352388</v>
+        <v>358295</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>13051.407407407407</v>
+        <v>12355</v>
       </c>
       <c r="K24" s="1">
         <f>(30*L6)-I24</f>
-        <v>-59213.13392857142</v>
+        <v>-65120.13392857142</v>
       </c>
       <c r="L24" s="4">
         <f>K24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>-3289.6185515873012</v>
+        <v>-3617.7852182539677</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -942,10 +942,16 @@
       <c r="A50" s="3">
         <v>42549</v>
       </c>
+      <c r="B50" s="1">
+        <v>5862</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>42550</v>
+      </c>
+      <c r="B51" s="1">
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Jun 30 to Jul 5 Steps
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -532,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,15 +608,15 @@
       </c>
       <c r="J6" s="1">
         <f>AVERAGE(B2:B16)</f>
-        <v>273629.875</v>
+        <v>285157.33333333331</v>
       </c>
       <c r="K6" s="1">
         <f>J6/4</f>
-        <v>68407.46875</v>
+        <v>71289.333333333328</v>
       </c>
       <c r="L6" s="1">
         <f>K6/7</f>
-        <v>9772.4955357142862</v>
+        <v>10184.190476190475</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -647,6 +647,9 @@
       <c r="A10" s="2">
         <v>42522</v>
       </c>
+      <c r="B10" s="1">
+        <v>377377</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -696,10 +699,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>42522</v>
+        <v>42552</v>
       </c>
       <c r="B23" s="1">
-        <v>13489</v>
+        <v>22431</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>10</v>
@@ -716,247 +719,183 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>42523</v>
+        <v>42553</v>
       </c>
       <c r="B24" s="1">
-        <v>11090</v>
+        <v>6609</v>
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>358295</v>
+        <v>61481</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>12355</v>
+        <v>10246.833333333334</v>
       </c>
       <c r="K24" s="1">
         <f>(30*L6)-I24</f>
-        <v>-65120.13392857142</v>
+        <v>244044.71428571426</v>
       </c>
       <c r="L24" s="4">
         <f>K24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>-3617.7852182539677</v>
+        <v>13558.039682539682</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>42524</v>
+        <v>42554</v>
       </c>
       <c r="B25" s="1">
-        <v>8509</v>
+        <v>3391</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>42525</v>
+        <v>42555</v>
       </c>
       <c r="B26" s="1">
-        <v>18480</v>
+        <v>16090</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>42526</v>
+        <v>42556</v>
       </c>
       <c r="B27" s="1">
-        <v>4784</v>
+        <v>9756</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>42527</v>
+        <v>42557</v>
       </c>
       <c r="B28" s="1">
-        <v>21982</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>42528</v>
-      </c>
-      <c r="B29" s="1">
-        <v>15662</v>
+        <v>42558</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>42529</v>
-      </c>
-      <c r="B30" s="1">
-        <v>6412</v>
+        <v>42559</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>42530</v>
-      </c>
-      <c r="B31" s="1">
-        <v>7959</v>
+        <v>42560</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>42531</v>
-      </c>
-      <c r="B32" s="1">
-        <v>2844</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42561</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>42532</v>
-      </c>
-      <c r="B33" s="1">
-        <v>13104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42562</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>42533</v>
-      </c>
-      <c r="B34" s="1">
-        <v>22915</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42563</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>42534</v>
-      </c>
-      <c r="B35" s="1">
-        <v>12396</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42564</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>42535</v>
-      </c>
-      <c r="B36" s="1">
-        <v>11692</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42565</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>42536</v>
-      </c>
-      <c r="B37" s="1">
-        <v>8262</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42566</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>42537</v>
-      </c>
-      <c r="B38" s="1">
-        <v>10959</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42567</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>42538</v>
-      </c>
-      <c r="B39" s="1">
-        <v>14493</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42568</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>42539</v>
-      </c>
-      <c r="B40" s="1">
-        <v>19776</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42569</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>42540</v>
-      </c>
-      <c r="B41" s="1">
-        <v>21227</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42570</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>42541</v>
-      </c>
-      <c r="B42" s="1">
-        <v>20933</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42571</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>42542</v>
-      </c>
-      <c r="B43" s="1">
-        <v>14891</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>42543</v>
-      </c>
-      <c r="B44" s="1">
-        <v>14193</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42573</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>42544</v>
-      </c>
-      <c r="B45" s="1">
-        <v>14976</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42574</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>42545</v>
-      </c>
-      <c r="B46" s="1">
-        <v>7515</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42575</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>42546</v>
-      </c>
-      <c r="B47" s="1">
-        <v>17364</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42576</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>42547</v>
-      </c>
-      <c r="B48" s="1">
-        <v>7425</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42577</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>42548</v>
-      </c>
-      <c r="B49" s="1">
-        <v>9056</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42578</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>42549</v>
-      </c>
-      <c r="B50" s="1">
-        <v>5862</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42579</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>42550</v>
-      </c>
-      <c r="B51" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42580</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>42551</v>
+        <v>42581</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>42582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Jul 6 Steps
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinguva\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinguva\Downloads\Fitbit Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Month" sheetId="2" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,23 +722,23 @@
         <v>42553</v>
       </c>
       <c r="B24" s="1">
-        <v>6609</v>
+        <v>7366</v>
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>61481</v>
+        <v>73000</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>10246.833333333334</v>
+        <v>10428.571428571429</v>
       </c>
       <c r="K24" s="1">
         <f>(30*L6)-I24</f>
-        <v>244044.71428571426</v>
+        <v>232525.71428571426</v>
       </c>
       <c r="L24" s="4">
         <f>K24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>13558.039682539682</v>
+        <v>12918.095238095237</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -746,7 +746,7 @@
         <v>42554</v>
       </c>
       <c r="B25" s="1">
-        <v>3391</v>
+        <v>4123</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -754,7 +754,7 @@
         <v>42555</v>
       </c>
       <c r="B26" s="1">
-        <v>16090</v>
+        <v>16421</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>42556</v>
       </c>
       <c r="B27" s="1">
-        <v>9756</v>
+        <v>9946</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -770,12 +770,15 @@
         <v>42557</v>
       </c>
       <c r="B28" s="1">
-        <v>3204</v>
+        <v>8593</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>42558</v>
+      </c>
+      <c r="B29" s="1">
+        <v>4120</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Jul 7 Steps
</commit_message>
<xml_diff>
--- a/Fbit - Steps- Weekly.xlsx
+++ b/Fbit - Steps- Weekly.xlsx
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,19 +726,19 @@
       </c>
       <c r="I24" s="1">
         <f xml:space="preserve"> SUM(B23:B52)</f>
-        <v>73000</v>
+        <v>78156</v>
       </c>
       <c r="J24" s="1">
         <f xml:space="preserve">  AVERAGE(B23:B52)</f>
-        <v>10428.571428571429</v>
+        <v>11165.142857142857</v>
       </c>
       <c r="K24" s="1">
         <f>(30*L6)-I24</f>
-        <v>232525.71428571426</v>
+        <v>227369.71428571426</v>
       </c>
       <c r="L24" s="4">
         <f>K24/(ROWS(A23:A52)-ROWS(A23:A34))</f>
-        <v>12918.095238095237</v>
+        <v>12631.650793650791</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
         <v>42558</v>
       </c>
       <c r="B29" s="1">
-        <v>4120</v>
+        <v>9276</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>